<commit_message>
début du jeu avec kable
</commit_message>
<xml_diff>
--- a/hepvs2020_ib/hepvs2020_ib_raw.xlsx
+++ b/hepvs2020_ib/hepvs2020_ib_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasbressoud/Documents/GitHub/r-projects/hepvs2020_ib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1411743A-F4CA-6E4A-8540-60D3089DA11D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2841FB-E6CD-D44E-A195-1BF4B2156F3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,13 +289,13 @@
     <t>m</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>o</t>
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>n_</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="158" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -631,13 +631,13 @@
         <v>88</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>